<commit_message>
Assistente - GEFIN v.2
</commit_message>
<xml_diff>
--- a/Planilhas/SESI_DR.xlsx
+++ b/Planilhas/SESI_DR.xlsx
@@ -73,7 +73,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="111" uniqueCount="63">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="100" uniqueCount="63">
   <si>
     <t>CNPJ</t>
   </si>
@@ -902,8 +902,8 @@
   </sheetPr>
   <dimension ref="A1:AS20"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
-      <selection activeCell="D17" sqref="D17"/>
+    <sheetView tabSelected="1" topLeftCell="A6" workbookViewId="0">
+      <selection activeCell="G16" sqref="G16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -1530,38 +1530,18 @@
       <c r="AR7" s="19"/>
       <c r="AS7" s="19"/>
     </row>
-    <row r="8" spans="1:45" s="20" customFormat="1" ht="104" x14ac:dyDescent="0.35">
-      <c r="A8" s="38" t="s">
-        <v>32</v>
-      </c>
+    <row r="8" spans="1:45" s="20" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="A8" s="38"/>
       <c r="B8" s="39"/>
-      <c r="C8" s="39" t="s">
-        <v>49</v>
-      </c>
-      <c r="D8" s="40">
-        <v>3388.34</v>
-      </c>
-      <c r="E8" s="41" t="s">
-        <v>50</v>
-      </c>
-      <c r="F8" s="42" t="s">
-        <v>51</v>
-      </c>
-      <c r="G8" s="39" t="s">
-        <v>52</v>
-      </c>
-      <c r="H8" s="42" t="s">
-        <v>53</v>
-      </c>
-      <c r="I8" s="43">
-        <v>43627</v>
-      </c>
-      <c r="J8" s="41" t="s">
-        <v>33</v>
-      </c>
-      <c r="K8" s="38" t="s">
-        <v>41</v>
-      </c>
+      <c r="C8" s="39"/>
+      <c r="D8" s="40"/>
+      <c r="E8" s="41"/>
+      <c r="F8" s="42"/>
+      <c r="G8" s="39"/>
+      <c r="H8" s="42"/>
+      <c r="I8" s="43"/>
+      <c r="J8" s="41"/>
+      <c r="K8" s="38"/>
       <c r="L8" s="44"/>
       <c r="M8" s="44"/>
       <c r="N8" s="45"/>
@@ -1571,36 +1551,22 @@
       <c r="R8" s="47"/>
       <c r="S8" s="46"/>
       <c r="T8" s="19"/>
-      <c r="U8" s="48">
-        <v>43628</v>
-      </c>
+      <c r="U8" s="48"/>
       <c r="V8" s="46"/>
-      <c r="W8" s="50" t="s">
-        <v>60</v>
-      </c>
+      <c r="W8" s="50"/>
       <c r="X8" s="44"/>
       <c r="Y8" s="46"/>
       <c r="Z8" s="46"/>
       <c r="AA8" s="44"/>
       <c r="AB8" s="44"/>
       <c r="AC8" s="44"/>
-      <c r="AD8" s="49">
-        <v>358</v>
-      </c>
-      <c r="AE8" s="46">
-        <v>1636</v>
-      </c>
-      <c r="AF8" s="48">
-        <v>43633</v>
-      </c>
-      <c r="AG8" s="46" t="s">
-        <v>34</v>
-      </c>
+      <c r="AD8" s="49"/>
+      <c r="AE8" s="46"/>
+      <c r="AF8" s="48"/>
+      <c r="AG8" s="46"/>
       <c r="AH8" s="46"/>
       <c r="AI8" s="46"/>
-      <c r="AJ8" s="46" t="s">
-        <v>35</v>
-      </c>
+      <c r="AJ8" s="46"/>
       <c r="AK8" s="19"/>
       <c r="AL8" s="19"/>
       <c r="AM8" s="19"/>
@@ -1896,10 +1862,9 @@
     <hyperlink ref="W4" r:id="rId3"/>
     <hyperlink ref="W6" r:id="rId4"/>
     <hyperlink ref="W7" r:id="rId5"/>
-    <hyperlink ref="W8" r:id="rId6"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" r:id="rId7"/>
-  <legacyDrawing r:id="rId8"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId6"/>
+  <legacyDrawing r:id="rId7"/>
 </worksheet>
 </file>
</xml_diff>